<commit_message>
Implementación pantalla ingreso de datos personales y bancarios
</commit_message>
<xml_diff>
--- a/test-data/credit_simulation_data.xlsx
+++ b/test-data/credit_simulation_data.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25915"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25917"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="53" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC335BAE-7B2A-463E-A364-EFF8EDF3B28D}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D14FAE4C-EF61-4D93-8889-6EC0B1F05FFD}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>user</t>
   </si>
@@ -43,6 +43,63 @@
   </si>
   <si>
     <t>month_of_grace</t>
+  </si>
+  <si>
+    <t>insurance</t>
+  </si>
+  <si>
+    <t>message_validation</t>
+  </si>
+  <si>
+    <t>ci_document</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>commune</t>
+  </si>
+  <si>
+    <t>bank</t>
+  </si>
+  <si>
+    <t>account_type</t>
+  </si>
+  <si>
+    <t>account_number</t>
+  </si>
+  <si>
+    <t>1400000</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>Sin meses de gracia</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>$ 1.400.000 - 54 Cuotas</t>
+  </si>
+  <si>
+    <t>PROVIDENCIA 123</t>
+  </si>
+  <si>
+    <t>Bio-Bio</t>
+  </si>
+  <si>
+    <t>Arauco</t>
+  </si>
+  <si>
+    <t>Itau</t>
+  </si>
+  <si>
+    <t>Cuenta Ahorro</t>
   </si>
 </sst>
 </file>
@@ -395,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -406,10 +463,16 @@
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,22 +488,76 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>132121109</v>
       </c>
       <c r="B2" s="1">
         <v>12345678</v>
       </c>
-      <c r="C2" s="1">
-        <v>1500000</v>
-      </c>
-      <c r="D2" s="1">
-        <v>40</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2">
+        <v>12345678</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2">
+        <v>123456789</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se realiza ajuste de lectura de datos desde excel, generación de reporte y ejecución de tests desde testng
</commit_message>
<xml_diff>
--- a/test-data/credit_simulation_data.xlsx
+++ b/test-data/credit_simulation_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25917"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="89" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D14FAE4C-EF61-4D93-8889-6EC0B1F05FFD}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9C21504-BD7B-4113-9E2B-A660608EC8B7}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>user</t>
   </si>
@@ -72,7 +72,10 @@
     <t>account_number</t>
   </si>
   <si>
-    <t>1400000</t>
+    <t>246757275</t>
+  </si>
+  <si>
+    <t>800000</t>
   </si>
   <si>
     <t>54</t>
@@ -84,7 +87,7 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>$ 1.400.000 - 54 Cuotas</t>
+    <t>$ 800.000 - 54 Cuotas</t>
   </si>
   <si>
     <t>PROVIDENCIA 123</t>
@@ -454,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -517,44 +520,44 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="1">
-        <v>132121109</v>
+      <c r="A2" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B2" s="1">
         <v>12345678</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2">
         <v>12345678</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N2">
         <v>123456789</v>

</xml_diff>

<commit_message>
Se realiza ajuste de lectura de datos desde excel, generación de reporte y ejecución de tests desde testng, se realiza implementación para cargar las fotos del anverso y reverso de cédula.
</commit_message>
<xml_diff>
--- a/test-data/credit_simulation_data.xlsx
+++ b/test-data/credit_simulation_data.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="93" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9C21504-BD7B-4113-9E2B-A660608EC8B7}"/>
+  <xr:revisionPtr revIDLastSave="130" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{182D9901-BBC4-4ABA-966D-38696B26457E}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>user</t>
   </si>
@@ -72,13 +72,22 @@
     <t>account_number</t>
   </si>
   <si>
-    <t>246757275</t>
-  </si>
-  <si>
-    <t>800000</t>
-  </si>
-  <si>
-    <t>54</t>
+    <t>assert_request_amount</t>
+  </si>
+  <si>
+    <t>assert_rut</t>
+  </si>
+  <si>
+    <t>55589143</t>
+  </si>
+  <si>
+    <t>QA2022</t>
+  </si>
+  <si>
+    <t>1500000</t>
+  </si>
+  <si>
+    <t>48</t>
   </si>
   <si>
     <t>Sin meses de gracia</t>
@@ -87,7 +96,7 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>$ 800.000 - 54 Cuotas</t>
+    <t>$ 1.500.000 - 48 Cuotas</t>
   </si>
   <si>
     <t>PROVIDENCIA 123</t>
@@ -103,19 +112,39 @@
   </si>
   <si>
     <t>Cuenta Ahorro</t>
+  </si>
+  <si>
+    <t>$ 1.500.000</t>
+  </si>
+  <si>
+    <t>5.558.914-3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -138,9 +167,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -159,7 +190,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -447,7 +478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -455,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -473,9 +504,11 @@
     <col min="12" max="12" width="14" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" customWidth="1"/>
     <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -518,49 +551,61 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="2">
+        <v>103238224</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2">
         <v>12345678</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2">
-        <v>12345678</v>
-      </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2">
-        <v>123456789</v>
+      <c r="O2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>